<commit_message>
Replaced old dashboard file with new updated one
Replaced old dashboard file with new updated one
</commit_message>
<xml_diff>
--- a/Project Tesla Sales 2016-2023 $TSLA.xlsx
+++ b/Project Tesla Sales 2016-2023 $TSLA.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/975a09036720cd9c/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/975a09036720cd9c/Desktop/TESLA PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{F6132C53-FD2A-4CB5-9E8C-3F82840914A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0311465E-D7AC-4718-AADE-E132E404B6A8}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="mX8Tfb2vlJCrflFHP8LcXoPE0qTz9SUcb83++siVv/3P2sIxXjL6EPjYnWxZqsuo1GbXO4tUpI1NOXKFrWV3XA==" workbookSaltValue="hfMJ9Uhx4rssOGO6sfZT4Q==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="8_{F6132C53-FD2A-4CB5-9E8C-3F82840914A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9106C191-63DF-4297-A0A3-6500B472102F}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="i/qn2R2hgLhNoCngq7/qam+EaBZTZlG+p0vNDm+qJxxHgXZde1Ga3JHAd+cn35+xWfo54P189AF/N3EYdfMG6A==" workbookSaltValue="4chWdGZTdYw/pX2yu0tRvw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2ECD4CDE-4E88-43D9-A109-5BF23C205DC5}"/>
   </bookViews>
@@ -26,15 +26,15 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
-    <pivotCache cacheId="1" r:id="rId4"/>
-    <pivotCache cacheId="2" r:id="rId5"/>
-    <pivotCache cacheId="3" r:id="rId6"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId5"/>
+    <pivotCache cacheId="8" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
       <x14:pivotCaches>
-        <pivotCache cacheId="4" r:id="rId7"/>
+        <pivotCache cacheId="9" r:id="rId7"/>
       </x14:pivotCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -505,8 +505,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Walutowy" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="44">
     <dxf>
@@ -769,9 +769,9 @@
   <colors>
     <mruColors>
       <color rgb="FF2D7CB1"/>
-      <color rgb="FF205D94"/>
       <color rgb="FF338DCB"/>
       <color rgb="FF215F9A"/>
+      <color rgb="FF205D94"/>
       <color rgb="FF2477DC"/>
       <color rgb="FF3280DE"/>
       <color rgb="FF4A90E2"/>
@@ -794,7 +794,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1935,7 +1935,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4025,7 +4025,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5636,7 +5636,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7078,7 +7078,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -11714,8 +11714,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1504950" y="0"/>
-          <a:ext cx="16211550" cy="1000125"/>
+          <a:off x="1509432" y="0"/>
+          <a:ext cx="17603321" cy="1023657"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11901,13 +11901,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>362218</xdr:colOff>
+      <xdr:colOff>2396</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>967</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>308555</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>520233</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>48592</xdr:rowOff>
     </xdr:to>
@@ -11924,8 +11924,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10947042" y="1879136"/>
-          <a:ext cx="2602605" cy="986710"/>
+          <a:off x="11654646" y="1905967"/>
+          <a:ext cx="2613337" cy="1000125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12064,13 +12064,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>187882</xdr:colOff>
+      <xdr:colOff>50303</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>38104</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>821275</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
@@ -12090,8 +12090,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6125132" y="1914525"/>
-          <a:ext cx="2411389" cy="1000125"/>
+          <a:off x="6633136" y="1914525"/>
+          <a:ext cx="2718306" cy="1000125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13027,13 +13027,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>594440</xdr:colOff>
+      <xdr:colOff>139362</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>53662</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>349253</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>89214</xdr:rowOff>
     </xdr:to>
@@ -13050,8 +13050,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11948240" y="2339662"/>
-          <a:ext cx="2158285" cy="416552"/>
+          <a:off x="11791612" y="2339662"/>
+          <a:ext cx="2305391" cy="416552"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13104,13 +13104,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>428626</xdr:colOff>
+      <xdr:colOff>291047</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>66039</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
+      <xdr:colOff>567271</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>104139</xdr:rowOff>
     </xdr:to>
@@ -13127,7 +13127,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7011459" y="2352039"/>
+          <a:off x="6873880" y="2352039"/>
           <a:ext cx="2223558" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13181,13 +13181,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>224371</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>93908</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>750463</xdr:colOff>
+      <xdr:colOff>612884</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>40246</xdr:rowOff>
     </xdr:to>
@@ -13204,8 +13204,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6734175" y="1998908"/>
-          <a:ext cx="2274463" cy="327338"/>
+          <a:off x="6807204" y="1998908"/>
+          <a:ext cx="2335847" cy="327338"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13251,13 +13251,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>482958</xdr:colOff>
+      <xdr:colOff>176051</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>93908</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>187815</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>338669</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>53661</xdr:rowOff>
     </xdr:to>
@@ -13274,8 +13274,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11067782" y="1972077"/>
-          <a:ext cx="2361125" cy="335387"/>
+          <a:off x="11828301" y="1998908"/>
+          <a:ext cx="2258118" cy="340753"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13397,6 +13397,962 @@
             </a:rPr>
             <a:t>$TSLA Total Growth</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>963083</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>74081</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>317499</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC93B3B5-4994-EB79-0070-60FB18814F52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17324916" y="15112998"/>
+          <a:ext cx="317500" cy="1164168"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" kern="1200"/>
+            <a:t>$</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" kern="1200">
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>TSLA Price</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>110066</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="pole tekstowe 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68F30E58-BA48-49DC-8275-F02974A83EE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1718733" y="14552083"/>
+          <a:ext cx="317500" cy="1358900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert270" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" kern="1200"/>
+            <a:t>GOLD &amp; INDEXES</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1400" kern="1200">
+            <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>110757</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>242112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>431948</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>11076</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75324082-FAC8-4321-AC81-17D19D4A3801}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{05273063-A62A-269A-03EF-12CFC5587E38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2248344" y="19059525"/>
+          <a:ext cx="4264098" cy="1164487"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="2D7CB1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" sx="104000" sy="104000" algn="ctr" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+          <a:softEdge rad="0"/>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="101600" prst="riblet"/>
+          <a:bevelB w="152400" h="50800" prst="softRound"/>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>126472</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>64057</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>465169</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>88605</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="TextBox 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91E1D7B7-C76B-EE33-7D50-E5E8BE40723E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5719641" y="18316615"/>
+          <a:ext cx="9608958" cy="401118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="215F9A"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="2000" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>INSIGHTS</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="2000">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>265817</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>44302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>265815</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>188285</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="pole tekstowe 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3FEF7E3-C8CD-B8E5-5F6E-BB2AE5108053}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2403404" y="19182907"/>
+          <a:ext cx="3942905" cy="897122"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Tesla's sales trend is strongly upward</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>, with consistent YOY growth, especially significant in 2022-2023, surpassing 600,000 units annually.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22152</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>44302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>708838</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="pole tekstowe 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C5434A5-6177-92E5-915D-789B309D3F58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8528199" y="19182907"/>
+          <a:ext cx="3798924" cy="708837"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="pl-PL" sz="3000" b="1" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>343344</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>44302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>110756</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="pole tekstowe 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42078DAA-5560-B02C-EA07-5A2A00C04830}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14630844" y="19182907"/>
+          <a:ext cx="3798924" cy="708837"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="pl-PL" sz="3000" b="1" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>265821</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>242112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>199366</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>11076</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3086E7F4-7B41-5653-9B02-638B369AEC12}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{05273063-A62A-269A-03EF-12CFC5587E38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8350995" y="19059525"/>
+          <a:ext cx="4264098" cy="1164487"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="2D7CB1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" sx="104000" sy="104000" algn="ctr" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+          <a:softEdge rad="0"/>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="101600" prst="riblet"/>
+          <a:bevelB w="152400" h="50800" prst="softRound"/>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>6</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>44302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>33231</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>188285</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="pole tekstowe 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E74E13D5-269E-481E-91BE-7567ACAEBEDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8506053" y="19182907"/>
+          <a:ext cx="3942905" cy="897122"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The Tesla Model Y has been the most popular model in the last three years</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>, capturing over 50% of Tesla's sales share in 2023.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>210437</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>242112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>587005</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>11076</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E556984-3831-436E-58B1-97E41ACF88BB}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{05273063-A62A-269A-03EF-12CFC5587E38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14497937" y="19059525"/>
+          <a:ext cx="4408080" cy="1164487"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="2D7CB1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" sx="104000" sy="104000" algn="ctr" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+          <a:softEdge rad="0"/>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="101600" prst="riblet"/>
+          <a:bevelB w="152400" h="50800" prst="softRound"/>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>299041</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>44302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>498400</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>188285</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="pole tekstowe 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5633D2F9-835E-1571-D181-45C4ACEE10AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14586541" y="19182907"/>
+          <a:ext cx="4230871" cy="897122"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>$TSLA stock price surged over the last</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>years</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>, closely aligning with rising vehicle</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>sales,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>especially the rapid growth of Model Y since</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>2020.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="Grandview" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -15390,7 +16346,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{25D486BC-FB3A-400C-B612-4596EF50E827}" name="PivotTable24" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Year">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{25D486BC-FB3A-400C-B612-4596EF50E827}" name="PivotTable24" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Year">
   <location ref="V21:Z29" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField numFmtId="165" showAll="0" defaultSubtotal="0">
@@ -15722,7 +16678,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1F71AC0-F1AD-4B2C-9BF7-3606BC11C8D1}" name="PivotSalesUSY" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Models">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1F71AC0-F1AD-4B2C-9BF7-3606BC11C8D1}" name="PivotSalesUSY" cacheId="7" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Models">
   <location ref="M21:R29" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisCol" allDrilled="1" subtotalTop="0" showAll="0" defaultAttributeDrillState="1">
@@ -15990,7 +16946,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{17AF247C-FB34-4895-A040-E170275DF452}" name="PivotSalesUST" cacheId="3" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Models">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{17AF247C-FB34-4895-A040-E170275DF452}" name="PivotSalesUST" cacheId="8" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Models">
   <location ref="C21:G29" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisCol" allDrilled="1" subtotalTop="0" showAll="0" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -16347,7 +17303,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3C59288C-C109-4160-88E7-8B3CA3A6F2AF}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3C59288C-C109-4160-88E7-8B3CA3A6F2AF}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="W21:AE26" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -16541,9 +17497,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -16581,7 +17537,7 @@
         <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
@@ -16687,7 +17643,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -16857,10 +17813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A20A7AD-9D63-47AE-8A3C-61E1BD2A5A74}">
-  <dimension ref="A1:Z106"/>
+  <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="AC89" sqref="AC89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16953,31 +17909,33 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
-      <c r="D21" t="s">
+      <c r="C21" s="28"/>
+      <c r="D21" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="N21" t="s">
+      <c r="M21" s="28"/>
+      <c r="N21" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21" s="28" t="s">
         <v>14</v>
       </c>
       <c r="V21" s="28" t="s">
@@ -17607,27 +18565,57 @@
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="30"/>
     </row>
-    <row r="101" spans="11:17" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97" s="17"/>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" s="17"/>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" s="17"/>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" s="17"/>
+    </row>
+    <row r="101" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="17"/>
       <c r="Q101" s="29"/>
     </row>
-    <row r="106" spans="11:17" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" s="17"/>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" s="17"/>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" s="30"/>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" s="30"/>
+    </row>
+    <row r="106" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="30"/>
       <c r="K106" s="29"/>
     </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" s="30"/>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A108" s="30"/>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A109" s="30"/>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110" s="30"/>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A111" s="30"/>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A112" s="30"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="R21">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F5EDC2F8-C44A-433A-B946-0BAFCDB28A60}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="R22:R29">
     <cfRule type="dataBar" priority="1">
       <dataBar>
@@ -17648,19 +18636,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F5EDC2F8-C44A-433A-B946-0BAFCDB28A60}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF63C384"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>R21</xm:sqref>
-        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
           <x14:cfRule type="dataBar" id="{E62F3E29-A431-4A81-85B1-C70B30F96282}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">

</xml_diff>